<commit_message>
bumped soft start time to 100ms
swapped 4.7uf for 22uf.
</commit_message>
<xml_diff>
--- a/Project Outputs for WordStorm/BOM/Bill of Materials-WordStorm.xlsx
+++ b/Project Outputs for WordStorm/BOM/Bill of Materials-WordStorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\WordStorm\Project Outputs for WordStorm\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E26027AA-E394-4521-AA89-F58B8E795F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7564054B-E683-4E1D-B393-D4CA6D221C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{2E36A71D-9211-4AE0-AA00-8BFF2A79B2F8}"/>
+    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{DDD143FC-0EB3-481A-9613-255AF01035D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WordStorm" sheetId="1" r:id="rId1"/>
@@ -77,40 +77,40 @@
     <t>C1, C4, C7, C9, C16, C17, C18, C19, C20, C36, C37, C38, C39, C40, C41, C43, C45, C48, C49, C50, C51, C52, C53</t>
   </si>
   <si>
+    <t>C2012X5R1V226M125AC</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 35V X5R 0805</t>
+  </si>
+  <si>
+    <t>C2, C5, C6, C8, C10, C11</t>
+  </si>
+  <si>
+    <t>GRM188R6YA106MA73D</t>
+  </si>
+  <si>
+    <t>10 µF ±20% 35V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>C3, C13</t>
+  </si>
+  <si>
+    <t>GRM1885C2A471JA01D</t>
+  </si>
+  <si>
+    <t>470 pF ±5% 100V Ceramic Capacitor C0G, NP0 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
     <t>GRM188R6YA475KE15D</t>
   </si>
   <si>
     <t>4.7 µF ±10% 35V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
   </si>
   <si>
-    <t>C2, C14</t>
-  </si>
-  <si>
-    <t>GRM188R6YA106MA73D</t>
-  </si>
-  <si>
-    <t>10 µF ±20% 35V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>C3, C13</t>
-  </si>
-  <si>
-    <t>C2012X5R1V226M125AC</t>
-  </si>
-  <si>
-    <t>CAP CER 22UF 35V X5R 0805</t>
-  </si>
-  <si>
-    <t>C5, C6, C8, C10, C11</t>
-  </si>
-  <si>
-    <t>GRM1885C2A471JA01D</t>
-  </si>
-  <si>
-    <t>470 pF ±5% 100V Ceramic Capacitor C0G, NP0 0603 (1608 Metric)</t>
-  </si>
-  <si>
-    <t>C12</t>
+    <t>C14</t>
   </si>
   <si>
     <t>GRM188R72A223KAC4D</t>
@@ -992,7 +992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28104AA6-94FE-40E3-9EEC-9621E4C910FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF646E68-7D22-4957-80CE-9C9175C69938}">
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1071,7 +1071,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed display connector wires.
</commit_message>
<xml_diff>
--- a/Project Outputs for WordStorm/BOM/Bill of Materials-WordStorm.xlsx
+++ b/Project Outputs for WordStorm/BOM/Bill of Materials-WordStorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\WordStorm\Project Outputs for WordStorm\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7564054B-E683-4E1D-B393-D4CA6D221C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C20F446C-937D-4C8F-B7DC-49010DDF60FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{DDD143FC-0EB3-481A-9613-255AF01035D9}"/>
+    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{27FE03CE-5F51-428A-A10E-6A2BDEFED7EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WordStorm" sheetId="1" r:id="rId1"/>
@@ -992,7 +992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF646E68-7D22-4957-80CE-9C9175C69938}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD9F18E-7485-4D99-8693-B6A0183AFFAF}">
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
added another draftman file
</commit_message>
<xml_diff>
--- a/Project Outputs for WordStorm/BOM/Bill of Materials-WordStorm.xlsx
+++ b/Project Outputs for WordStorm/BOM/Bill of Materials-WordStorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\WordStorm\Project Outputs for WordStorm\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A35A75DF-5B77-46F3-9DB4-11F4E0285BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2300EDF4-C078-452B-A4A3-4176F80CBDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="2775" windowWidth="21600" windowHeight="13065" xr2:uid="{A9E9E034-B60C-4E49-8FF6-284D37D8F918}"/>
+    <workbookView xWindow="3615" yWindow="2775" windowWidth="21600" windowHeight="13065" xr2:uid="{5A913B72-C91A-4835-BAB8-A559B6CE0A00}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WordStorm" sheetId="1" r:id="rId1"/>
@@ -992,7 +992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437372D4-968E-4737-99EF-98275B8EFE93}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C4E01A-09E0-46F2-8C77-B0B91FCFCEF8}">
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>